<commit_message>
added information about source plate
</commit_message>
<xml_diff>
--- a/metadata/drug_treatment_log.xlsx
+++ b/metadata/drug_treatment_log.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C77B1580-F794-48B8-9573-720B338EEBB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A47D326-A0ED-4DE5-ACD7-5769A946BE26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10996" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="125">
   <si>
     <t>CL1</t>
   </si>
@@ -352,6 +352,60 @@
   </si>
   <si>
     <t>start_data</t>
+  </si>
+  <si>
+    <t>1MSP009</t>
+  </si>
+  <si>
+    <t>2MSP002</t>
+  </si>
+  <si>
+    <t>1MSP010</t>
+  </si>
+  <si>
+    <t>2MSP003</t>
+  </si>
+  <si>
+    <t>1MSP011</t>
+  </si>
+  <si>
+    <t>2MSP004</t>
+  </si>
+  <si>
+    <t>1MSP012</t>
+  </si>
+  <si>
+    <t>2MSP005</t>
+  </si>
+  <si>
+    <t>1MSP013</t>
+  </si>
+  <si>
+    <t>2MSP006</t>
+  </si>
+  <si>
+    <t>1MSP014</t>
+  </si>
+  <si>
+    <t>2MSP007</t>
+  </si>
+  <si>
+    <t>1MSP015</t>
+  </si>
+  <si>
+    <t>2MSP008</t>
+  </si>
+  <si>
+    <t>source1</t>
+  </si>
+  <si>
+    <t>source2</t>
+  </si>
+  <si>
+    <t>MSP_layout</t>
+  </si>
+  <si>
+    <t>190806_NewMSP_Layout</t>
   </si>
 </sst>
 </file>
@@ -401,7 +455,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -415,6 +469,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -859,11 +916,11 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:V30"/>
+  <dimension ref="A1:Y30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="3" topLeftCell="D1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="I2" sqref="I2"/>
+      <selection pane="topRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -890,13 +947,13 @@
     <col min="21" max="21" width="16.73046875" style="2" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="16.1328125" style="2" bestFit="1" customWidth="1"/>
     <col min="23" max="24" width="9.06640625" style="1"/>
-    <col min="25" max="25" width="87.86328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="23.265625" bestFit="1" customWidth="1"/>
     <col min="26" max="28" width="9.06640625" style="1"/>
     <col min="29" max="29" width="27.73046875" style="1" bestFit="1" customWidth="1"/>
     <col min="30" max="16384" width="9.06640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>28</v>
       </c>
@@ -963,8 +1020,17 @@
       <c r="V1" s="2" t="s">
         <v>20</v>
       </c>
+      <c r="W1" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="X1" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>123</v>
+      </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -1016,23 +1082,32 @@
       <c r="Q2" s="6">
         <v>1218</v>
       </c>
-      <c r="R2" s="2">
+      <c r="R2" s="6">
         <v>2</v>
       </c>
-      <c r="S2" s="3">
+      <c r="S2" s="7">
         <v>1015</v>
       </c>
-      <c r="T2" s="2">
+      <c r="T2" s="6">
         <v>1148</v>
       </c>
-      <c r="U2" s="2">
+      <c r="U2" s="6">
         <v>1155</v>
       </c>
-      <c r="V2" s="2">
+      <c r="V2" s="6">
         <v>1315</v>
       </c>
+      <c r="W2" t="s">
+        <v>107</v>
+      </c>
+      <c r="X2" t="s">
+        <v>108</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>124</v>
+      </c>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -1084,23 +1159,32 @@
       <c r="Q3" s="6">
         <v>1730</v>
       </c>
-      <c r="R3" s="2">
+      <c r="R3" s="6">
         <v>3</v>
       </c>
-      <c r="S3" s="3">
+      <c r="S3" s="7">
         <v>1607</v>
       </c>
-      <c r="T3" s="2">
+      <c r="T3" s="6">
         <v>1732</v>
       </c>
-      <c r="U3" s="2">
+      <c r="U3" s="6">
         <v>1900</v>
       </c>
-      <c r="V3" s="2">
+      <c r="V3" s="6">
         <v>2009</v>
       </c>
+      <c r="W3" t="s">
+        <v>107</v>
+      </c>
+      <c r="X3" t="s">
+        <v>108</v>
+      </c>
+      <c r="Y3" t="s">
+        <v>124</v>
+      </c>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A4" s="1">
         <v>1</v>
       </c>
@@ -1152,23 +1236,32 @@
       <c r="Q4" s="6">
         <v>1730</v>
       </c>
-      <c r="R4" s="2">
+      <c r="R4" s="6">
         <v>3</v>
       </c>
-      <c r="S4" s="3">
+      <c r="S4" s="7">
         <v>1740</v>
       </c>
-      <c r="T4" s="2">
+      <c r="T4" s="6">
         <v>1946</v>
       </c>
-      <c r="U4" s="2">
+      <c r="U4" s="6">
         <v>1912</v>
       </c>
-      <c r="V4" s="2">
+      <c r="V4" s="6">
         <v>2115</v>
       </c>
+      <c r="W4" t="s">
+        <v>107</v>
+      </c>
+      <c r="X4" t="s">
+        <v>108</v>
+      </c>
+      <c r="Y4" t="s">
+        <v>124</v>
+      </c>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A5" s="1">
         <v>2</v>
       </c>
@@ -1220,23 +1313,32 @@
       <c r="Q5" s="6">
         <v>1451</v>
       </c>
-      <c r="R5" s="2">
+      <c r="R5" s="6">
         <v>2</v>
       </c>
-      <c r="S5" s="3" t="s">
+      <c r="S5" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="T5" s="2">
+      <c r="T5" s="6">
         <v>1046</v>
       </c>
-      <c r="U5" s="2">
+      <c r="U5" s="6">
         <v>1415</v>
       </c>
-      <c r="V5" s="2">
+      <c r="V5" s="6">
         <v>1519</v>
       </c>
+      <c r="W5" t="s">
+        <v>109</v>
+      </c>
+      <c r="X5" t="s">
+        <v>110</v>
+      </c>
+      <c r="Y5" t="s">
+        <v>124</v>
+      </c>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A6" s="1">
         <v>2</v>
       </c>
@@ -1288,23 +1390,32 @@
       <c r="Q6" s="6">
         <v>1451</v>
       </c>
-      <c r="R6" s="2">
+      <c r="R6" s="6">
         <v>2</v>
       </c>
-      <c r="S6" s="3">
+      <c r="S6" s="7">
         <v>1046</v>
       </c>
-      <c r="T6" s="2">
+      <c r="T6" s="6">
         <v>1140</v>
       </c>
-      <c r="U6" s="2">
+      <c r="U6" s="6">
         <v>1519</v>
       </c>
-      <c r="V6" s="2">
+      <c r="V6" s="6">
         <v>1606</v>
       </c>
+      <c r="W6" t="s">
+        <v>109</v>
+      </c>
+      <c r="X6" t="s">
+        <v>110</v>
+      </c>
+      <c r="Y6" t="s">
+        <v>124</v>
+      </c>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A7" s="1">
         <v>2</v>
       </c>
@@ -1356,23 +1467,32 @@
       <c r="Q7" s="6">
         <v>1451</v>
       </c>
-      <c r="R7" s="2">
+      <c r="R7" s="6">
         <v>2</v>
       </c>
-      <c r="S7" s="3">
+      <c r="S7" s="7">
         <v>1140</v>
       </c>
-      <c r="T7" s="2">
+      <c r="T7" s="6">
         <v>1230</v>
       </c>
-      <c r="U7" s="2">
+      <c r="U7" s="6">
         <v>1641</v>
       </c>
-      <c r="V7" s="2">
+      <c r="V7" s="6">
         <v>1730</v>
       </c>
+      <c r="W7" t="s">
+        <v>109</v>
+      </c>
+      <c r="X7" t="s">
+        <v>110</v>
+      </c>
+      <c r="Y7" t="s">
+        <v>124</v>
+      </c>
     </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A8" s="1">
         <v>3</v>
       </c>
@@ -1424,23 +1544,32 @@
       <c r="Q8" s="6">
         <v>1335</v>
       </c>
-      <c r="R8" s="2">
+      <c r="R8" s="6">
         <v>2</v>
       </c>
-      <c r="S8" s="3" t="s">
+      <c r="S8" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="T8" s="2">
+      <c r="T8" s="6">
         <v>1512</v>
       </c>
-      <c r="U8" s="2">
+      <c r="U8" s="6">
         <v>1513</v>
       </c>
-      <c r="V8" s="2">
+      <c r="V8" s="6">
         <v>1610</v>
       </c>
+      <c r="W8" t="s">
+        <v>111</v>
+      </c>
+      <c r="X8" t="s">
+        <v>112</v>
+      </c>
+      <c r="Y8" t="s">
+        <v>124</v>
+      </c>
     </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A9" s="1">
         <v>3</v>
       </c>
@@ -1492,23 +1621,32 @@
       <c r="Q9" s="6">
         <v>1335</v>
       </c>
-      <c r="R9" s="2">
+      <c r="R9" s="6">
         <v>2</v>
       </c>
-      <c r="S9" s="3" t="s">
+      <c r="S9" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="T9" s="2">
+      <c r="T9" s="6">
         <v>1804</v>
       </c>
-      <c r="U9" s="2">
+      <c r="U9" s="6">
         <v>1805</v>
       </c>
-      <c r="V9" s="2">
+      <c r="V9" s="6">
         <v>1906</v>
       </c>
+      <c r="W9" t="s">
+        <v>111</v>
+      </c>
+      <c r="X9" t="s">
+        <v>112</v>
+      </c>
+      <c r="Y9" t="s">
+        <v>124</v>
+      </c>
     </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A10" s="1">
         <v>3</v>
       </c>
@@ -1560,23 +1698,32 @@
       <c r="Q10" s="6">
         <v>1335</v>
       </c>
-      <c r="R10" s="2">
+      <c r="R10" s="6">
         <v>2</v>
       </c>
-      <c r="S10" s="3" t="s">
+      <c r="S10" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="T10" s="2">
+      <c r="T10" s="6">
         <v>1127</v>
       </c>
-      <c r="U10" s="2">
+      <c r="U10" s="6">
         <v>1127</v>
       </c>
-      <c r="V10" s="2">
+      <c r="V10" s="6">
         <v>1219</v>
       </c>
+      <c r="W10" t="s">
+        <v>111</v>
+      </c>
+      <c r="X10" t="s">
+        <v>112</v>
+      </c>
+      <c r="Y10" t="s">
+        <v>124</v>
+      </c>
     </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A11" s="1">
         <v>4</v>
       </c>
@@ -1628,23 +1775,32 @@
       <c r="Q11" s="6">
         <v>1233</v>
       </c>
-      <c r="R11" s="2">
+      <c r="R11" s="6">
         <v>2</v>
       </c>
-      <c r="S11" s="3" t="s">
+      <c r="S11" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="T11" s="2">
+      <c r="T11" s="6">
         <v>1136</v>
       </c>
-      <c r="U11" s="2">
+      <c r="U11" s="6">
         <v>1330</v>
       </c>
-      <c r="V11" s="2">
+      <c r="V11" s="6">
         <v>1426</v>
       </c>
+      <c r="W11" t="s">
+        <v>113</v>
+      </c>
+      <c r="X11" t="s">
+        <v>114</v>
+      </c>
+      <c r="Y11" t="s">
+        <v>124</v>
+      </c>
     </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A12" s="1">
         <v>4</v>
       </c>
@@ -1696,23 +1852,32 @@
       <c r="Q12" s="6">
         <v>1648</v>
       </c>
-      <c r="R12" s="2">
+      <c r="R12" s="6">
         <v>3</v>
       </c>
-      <c r="S12" s="3" t="s">
+      <c r="S12" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="T12" s="2">
+      <c r="T12" s="6">
         <v>1514</v>
       </c>
-      <c r="U12" s="2">
+      <c r="U12" s="6">
         <v>1516</v>
       </c>
-      <c r="V12" s="2">
+      <c r="V12" s="6">
         <v>1607</v>
       </c>
+      <c r="W12" t="s">
+        <v>113</v>
+      </c>
+      <c r="X12" t="s">
+        <v>114</v>
+      </c>
+      <c r="Y12" t="s">
+        <v>124</v>
+      </c>
     </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A13" s="1">
         <v>4</v>
       </c>
@@ -1764,23 +1929,32 @@
       <c r="Q13" s="6">
         <v>1233</v>
       </c>
-      <c r="R13" s="2">
+      <c r="R13" s="6">
         <v>2</v>
       </c>
-      <c r="S13" s="3" t="s">
+      <c r="S13" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="T13" s="2">
+      <c r="T13" s="6">
         <v>1230</v>
       </c>
-      <c r="U13" s="2">
+      <c r="U13" s="6">
         <v>1429</v>
       </c>
-      <c r="V13" s="2">
+      <c r="V13" s="6">
         <v>1515</v>
       </c>
+      <c r="W13" t="s">
+        <v>113</v>
+      </c>
+      <c r="X13" t="s">
+        <v>114</v>
+      </c>
+      <c r="Y13" t="s">
+        <v>124</v>
+      </c>
     </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A14" s="1">
         <v>5</v>
       </c>
@@ -1832,23 +2006,32 @@
       <c r="Q14" s="6">
         <v>1354</v>
       </c>
-      <c r="R14" s="2">
+      <c r="R14" s="6">
         <v>2</v>
       </c>
-      <c r="S14" s="3" t="s">
+      <c r="S14" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="T14" s="2">
+      <c r="T14" s="6">
         <v>1128</v>
       </c>
-      <c r="U14" s="2">
+      <c r="U14" s="6">
         <v>1450</v>
       </c>
-      <c r="V14" s="2">
+      <c r="V14" s="6">
         <v>1536</v>
       </c>
+      <c r="W14" t="s">
+        <v>115</v>
+      </c>
+      <c r="X14" t="s">
+        <v>116</v>
+      </c>
+      <c r="Y14" t="s">
+        <v>124</v>
+      </c>
     </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A15" s="1">
         <v>5</v>
       </c>
@@ -1900,23 +2083,32 @@
       <c r="Q15" s="6">
         <v>1354</v>
       </c>
-      <c r="R15" s="2">
+      <c r="R15" s="6">
         <v>2</v>
       </c>
-      <c r="S15" s="3" t="s">
+      <c r="S15" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="T15" s="2">
+      <c r="T15" s="6">
         <v>1223</v>
       </c>
-      <c r="U15" s="2">
+      <c r="U15" s="6">
         <v>1539</v>
       </c>
-      <c r="V15" s="2">
+      <c r="V15" s="6">
         <v>1620</v>
       </c>
+      <c r="W15" t="s">
+        <v>115</v>
+      </c>
+      <c r="X15" t="s">
+        <v>116</v>
+      </c>
+      <c r="Y15" t="s">
+        <v>124</v>
+      </c>
     </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A16" s="1">
         <v>5</v>
       </c>
@@ -1968,23 +2160,32 @@
       <c r="Q16" s="6">
         <v>1354</v>
       </c>
-      <c r="R16" s="2">
+      <c r="R16" s="6">
         <v>2</v>
       </c>
-      <c r="S16" s="3" t="s">
+      <c r="S16" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="T16" s="2">
+      <c r="T16" s="6">
         <v>1325</v>
       </c>
-      <c r="U16" s="2">
+      <c r="U16" s="6">
         <v>1657</v>
       </c>
-      <c r="V16" s="2">
+      <c r="V16" s="6">
         <v>1755</v>
       </c>
+      <c r="W16" t="s">
+        <v>115</v>
+      </c>
+      <c r="X16" t="s">
+        <v>116</v>
+      </c>
+      <c r="Y16" t="s">
+        <v>124</v>
+      </c>
     </row>
-    <row r="17" spans="1:22" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A17" s="1">
         <v>6</v>
       </c>
@@ -2036,23 +2237,32 @@
       <c r="Q17" s="6">
         <v>1236</v>
       </c>
-      <c r="R17" s="2">
+      <c r="R17" s="6">
         <v>2</v>
       </c>
-      <c r="S17" s="3" t="s">
+      <c r="S17" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="T17" s="2">
+      <c r="T17" s="6">
         <v>1105</v>
       </c>
-      <c r="U17" s="2">
+      <c r="U17" s="6">
         <v>1347</v>
       </c>
-      <c r="V17" s="2">
+      <c r="V17" s="6">
         <v>1435</v>
       </c>
+      <c r="W17" t="s">
+        <v>117</v>
+      </c>
+      <c r="X17" t="s">
+        <v>118</v>
+      </c>
+      <c r="Y17" t="s">
+        <v>124</v>
+      </c>
     </row>
-    <row r="18" spans="1:22" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A18" s="1">
         <v>6</v>
       </c>
@@ -2104,23 +2314,32 @@
       <c r="Q18" s="6">
         <v>1236</v>
       </c>
-      <c r="R18" s="2">
+      <c r="R18" s="6">
         <v>2</v>
       </c>
-      <c r="S18" s="3" t="s">
+      <c r="S18" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="T18" s="2">
+      <c r="T18" s="6">
         <v>1151</v>
       </c>
-      <c r="U18" s="2">
+      <c r="U18" s="6">
         <v>1437</v>
       </c>
-      <c r="V18" s="2">
+      <c r="V18" s="6">
         <v>1519</v>
       </c>
+      <c r="W18" t="s">
+        <v>117</v>
+      </c>
+      <c r="X18" t="s">
+        <v>118</v>
+      </c>
+      <c r="Y18" t="s">
+        <v>124</v>
+      </c>
     </row>
-    <row r="19" spans="1:22" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A19" s="1">
         <v>6</v>
       </c>
@@ -2172,23 +2391,32 @@
       <c r="Q19" s="6">
         <v>1236</v>
       </c>
-      <c r="R19" s="2">
+      <c r="R19" s="6">
         <v>2</v>
       </c>
-      <c r="S19" s="3" t="s">
+      <c r="S19" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="T19" s="2">
+      <c r="T19" s="6">
         <v>1239</v>
       </c>
-      <c r="U19" s="2">
+      <c r="U19" s="6">
         <v>1529</v>
       </c>
-      <c r="V19" s="2">
+      <c r="V19" s="6">
         <v>1612</v>
       </c>
+      <c r="W19" t="s">
+        <v>117</v>
+      </c>
+      <c r="X19" t="s">
+        <v>118</v>
+      </c>
+      <c r="Y19" t="s">
+        <v>124</v>
+      </c>
     </row>
-    <row r="20" spans="1:22" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A20" s="1">
         <v>7</v>
       </c>
@@ -2240,23 +2468,32 @@
       <c r="Q20" s="6">
         <v>1422</v>
       </c>
-      <c r="R20" s="2">
+      <c r="R20" s="6">
         <v>2</v>
       </c>
-      <c r="S20" s="3" t="s">
+      <c r="S20" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="T20" s="2">
+      <c r="T20" s="6">
         <v>1108</v>
       </c>
-      <c r="U20" s="2">
+      <c r="U20" s="6">
         <v>1422</v>
       </c>
-      <c r="V20" s="2">
+      <c r="V20" s="6">
         <v>1500</v>
       </c>
+      <c r="W20" t="s">
+        <v>119</v>
+      </c>
+      <c r="X20" t="s">
+        <v>120</v>
+      </c>
+      <c r="Y20" t="s">
+        <v>124</v>
+      </c>
     </row>
-    <row r="21" spans="1:22" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A21" s="1">
         <v>7</v>
       </c>
@@ -2308,23 +2545,32 @@
       <c r="Q21" s="6">
         <v>1422</v>
       </c>
-      <c r="R21" s="2">
+      <c r="R21" s="6">
         <v>2</v>
       </c>
-      <c r="S21" s="3" t="s">
+      <c r="S21" s="7" t="s">
         <v>100</v>
       </c>
-      <c r="T21" s="2">
+      <c r="T21" s="6">
         <v>1153</v>
       </c>
-      <c r="U21" s="2">
+      <c r="U21" s="6">
         <v>1517</v>
       </c>
-      <c r="V21" s="2">
+      <c r="V21" s="6">
         <v>1554</v>
       </c>
+      <c r="W21" t="s">
+        <v>119</v>
+      </c>
+      <c r="X21" t="s">
+        <v>120</v>
+      </c>
+      <c r="Y21" t="s">
+        <v>124</v>
+      </c>
     </row>
-    <row r="22" spans="1:22" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A22" s="1">
         <v>7</v>
       </c>
@@ -2376,41 +2622,50 @@
       <c r="Q22" s="6">
         <v>1422</v>
       </c>
-      <c r="R22" s="2">
+      <c r="R22" s="6">
         <v>2</v>
       </c>
-      <c r="S22" s="3" t="s">
+      <c r="S22" s="7" t="s">
         <v>101</v>
       </c>
-      <c r="T22" s="2">
+      <c r="T22" s="6">
         <v>1235</v>
       </c>
-      <c r="U22" s="2">
+      <c r="U22" s="6">
         <v>1602</v>
       </c>
-      <c r="V22" s="2">
+      <c r="V22" s="6">
         <v>1645</v>
       </c>
+      <c r="W22" t="s">
+        <v>119</v>
+      </c>
+      <c r="X22" t="s">
+        <v>120</v>
+      </c>
+      <c r="Y22" t="s">
+        <v>124</v>
+      </c>
     </row>
-    <row r="24" spans="1:22" ht="15.4" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:25" ht="15.4" x14ac:dyDescent="0.45">
       <c r="C24" s="5"/>
     </row>
-    <row r="25" spans="1:22" ht="15.4" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:25" ht="15.4" x14ac:dyDescent="0.45">
       <c r="C25" s="5"/>
     </row>
-    <row r="26" spans="1:22" ht="15.4" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:25" ht="15.4" x14ac:dyDescent="0.45">
       <c r="C26" s="5"/>
     </row>
-    <row r="27" spans="1:22" ht="15.4" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:25" ht="15.4" x14ac:dyDescent="0.45">
       <c r="C27" s="5"/>
     </row>
-    <row r="28" spans="1:22" ht="15.4" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:25" ht="15.4" x14ac:dyDescent="0.45">
       <c r="C28" s="5"/>
     </row>
-    <row r="29" spans="1:22" ht="15.4" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:25" ht="15.4" x14ac:dyDescent="0.45">
       <c r="C29" s="5"/>
     </row>
-    <row r="30" spans="1:22" ht="15.4" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:25" ht="15.4" x14ac:dyDescent="0.45">
       <c r="C30" s="5"/>
     </row>
   </sheetData>

</xml_diff>